<commit_message>
Add excel for model evaluation
</commit_message>
<xml_diff>
--- a/evaluations/Models.xlsx
+++ b/evaluations/Models.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Model ID</t>
   </si>
@@ -51,6 +51,75 @@
   </si>
   <si>
     <t>short model name</t>
+  </si>
+  <si>
+    <t>screen</t>
+  </si>
+  <si>
+    <t>batch size</t>
+  </si>
+  <si>
+    <t>embedding size</t>
+  </si>
+  <si>
+    <t>epochs</t>
+  </si>
+  <si>
+    <t>latent dim</t>
+  </si>
+  <si>
+    <t>max decoder seq len</t>
+  </si>
+  <si>
+    <t>max decoder tokens</t>
+  </si>
+  <si>
+    <t>max encoder seq len</t>
+  </si>
+  <si>
+    <t>max encoder tokens</t>
+  </si>
+  <si>
+    <t>max num samples</t>
+  </si>
+  <si>
+    <t>max num words</t>
+  </si>
+  <si>
+    <t>max sentences</t>
+  </si>
+  <si>
+    <t>max seq len</t>
+  </si>
+  <si>
+    <t>p dense dropout</t>
+  </si>
+  <si>
+    <t>variant</t>
+  </si>
+  <si>
+    <t>Bemerkung</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>val loss</t>
+  </si>
+  <si>
+    <t>val bleu</t>
+  </si>
+  <si>
+    <t>train bleu</t>
+  </si>
+  <si>
+    <t>train loss</t>
+  </si>
+  <si>
+    <t>char keras tut ohne dropout</t>
+  </si>
+  <si>
+    <t>char keras tut mit dropout</t>
   </si>
 </sst>
 </file>
@@ -115,13 +184,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -402,24 +470,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:H9"/>
+  <dimension ref="A4:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="58" customWidth="1"/>
+    <col min="6" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="9" max="9" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
+        <f>"srun --pty --ntasks=1 --cpus-per-task=2 --mem=16G --gres=gpu:1 bash"</f>
+        <v>srun --pty --ntasks=1 --cpus-per-task=2 --mem=16G --gres=gpu:1 bash</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -435,14 +515,36 @@
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -461,13 +563,93 @@
         <f>CONCATENATE("persistentModel_",D9)</f>
         <v>persistentModel_einardan_seq2seq1</v>
       </c>
-      <c r="G9" s="3" t="str">
-        <f>CONCATENATE("nvidia-docker build -f ",B9," -t ",B9," .")</f>
-        <v>nvidia-docker build -f _64_100_15_256_3633_3950_2000000_20000_1000_100_321_307_0.8_char___tf -t _64_100_15_256_3633_3950_2000000_20000_1000_100_321_307_0.8_char___tf .</v>
-      </c>
-      <c r="H9" s="3" t="str">
+      <c r="G9" s="1" t="str">
+        <f>CONCATENATE("hofernicModel",B9)</f>
+        <v>hofernicModel_64_100_15_256_3633_3950_2000000_20000_1000_100_321_307_0.8_char___tf</v>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f>CONCATENATE("nvidia-docker build -f ",C9," -t ",E9," .")</f>
+        <v>nvidia-docker build -f Dockerfile_64_100_15_256_3633_3950_2000000_20000_1000_100_321_307_0.8_char___tf.prod -t hofernic_model_einardan_seq2seq1 .</v>
+      </c>
+      <c r="I9" s="4" t="str">
         <f>CONCATENATE("nvidia-docker run --rm -v ~/data/",F9,":/persistent -it ",E9,)</f>
         <v>nvidia-docker run --rm -v ~/data/persistentModel_einardan_seq2seq1:/persistent -it hofernic_model_einardan_seq2seq1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>